<commit_message>
updated calib sheet and elec calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/EDLE/Electricity Dispatch Logit Exponent.xlsx
+++ b/InputData/elec/EDLE/Electricity Dispatch Logit Exponent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaggarwal/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/MI/elec/EDLE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Michigan\MI-EPS\InputData\elec\EDLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67C24F2F-90F1-124C-9F62-29F870DD593E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2B3864-2387-46B5-9E76-040558287F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="1770" yWindow="720" windowWidth="18585" windowHeight="16635" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -455,11 +455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -470,7 +470,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -478,42 +478,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -530,17 +530,17 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -548,12 +548,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>-3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>